<commit_message>
kNN classifier with Mahalanobis distance is added.
</commit_message>
<xml_diff>
--- a/SPA2019/Database_description.xlsx
+++ b/SPA2019/Database_description.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Troparion\Interspeech2019_database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Troparion\SPA2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11880" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pathology" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="5">
   <si>
     <t>Sex</t>
   </si>
@@ -297,8 +297,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица2" displayName="Таблица2" ref="A1:C40" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:C40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица2" displayName="Таблица2" ref="A1:C38" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:C38"/>
   <tableColumns count="3">
     <tableColumn id="1" name="ID" dataDxfId="2"/>
     <tableColumn id="3" name="Age" dataDxfId="1"/>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,10 +760,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD41"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,43 +1049,43 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B26" s="8">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B27" s="8">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B28" s="8">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B29" s="8">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>2</v>
@@ -1093,21 +1093,21 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B30" s="8">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B31" s="8">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>2</v>
@@ -1115,10 +1115,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B32" s="8">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>2</v>
@@ -1126,21 +1126,21 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B33" s="8">
-        <v>55</v>
-      </c>
-      <c r="C33" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B34" s="8">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>2</v>
@@ -1148,10 +1148,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B35" s="8">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>2</v>
@@ -1159,10 +1159,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B36" s="8">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>2</v>
@@ -1170,45 +1170,23 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B37" s="8">
-        <v>39</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>2</v>
+        <v>80</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B38" s="8">
         <v>57</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
-        <v>107</v>
-      </c>
-      <c r="B39" s="8">
-        <v>80</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
-        <v>109</v>
-      </c>
-      <c r="B40" s="8">
-        <v>57</v>
-      </c>
-      <c r="C40" s="4" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Performance analysis of LDA and kNN classifiers added.
</commit_message>
<xml_diff>
--- a/SPA2019/Database_description.xlsx
+++ b/SPA2019/Database_description.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="5">
   <si>
     <t>Sex</t>
   </si>
@@ -46,7 +46,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,6 +59,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -106,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -130,6 +138,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -285,8 +299,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:C15" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:C15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:C16" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:C16"/>
   <tableColumns count="3">
     <tableColumn id="1" name="ID" dataDxfId="7"/>
     <tableColumn id="4" name="Age" dataDxfId="6"/>
@@ -297,8 +311,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица2" displayName="Таблица2" ref="A1:C38" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:C38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица2" displayName="Таблица2" ref="A1:C40" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:C40"/>
   <tableColumns count="3">
     <tableColumn id="1" name="ID" dataDxfId="2"/>
     <tableColumn id="3" name="Age" dataDxfId="1"/>
@@ -571,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,6 +763,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>68</v>
+      </c>
+      <c r="B16" s="3">
+        <v>40</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -760,10 +785,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,66 +1073,66 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>67</v>
-      </c>
-      <c r="B26" s="8">
-        <v>18</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>2</v>
+      <c r="A26" s="9">
+        <v>65</v>
+      </c>
+      <c r="B26" s="10">
+        <v>48</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B27" s="8">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B28" s="8">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B29" s="8">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>83</v>
-      </c>
-      <c r="B30" s="8">
-        <v>30</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>2</v>
+      <c r="A30" s="9">
+        <v>79</v>
+      </c>
+      <c r="B30" s="10">
+        <v>21</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B31" s="8">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>2</v>
@@ -1115,10 +1140,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B32" s="8">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>2</v>
@@ -1126,21 +1151,21 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B33" s="8">
-        <v>45</v>
-      </c>
-      <c r="C33" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B34" s="8">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>2</v>
@@ -1148,10 +1173,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B35" s="8">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>2</v>
@@ -1159,10 +1184,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B36" s="8">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>2</v>
@@ -1170,23 +1195,45 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B37" s="8">
-        <v>80</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B38" s="8">
         <v>57</v>
       </c>
       <c r="C38" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>107</v>
+      </c>
+      <c r="B39" s="8">
+        <v>80</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>109</v>
+      </c>
+      <c r="B40" s="8">
+        <v>57</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>